<commit_message>
Updated relevant SQL and table files
</commit_message>
<xml_diff>
--- a/Tableau Table 1.xlsx
+++ b/Tableau Table 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssoor\Desktop\DA projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2E3ACA5-3881-4F50-BEBA-1395561E46B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF8FE48-4275-4402-A6D9-22D092EDD282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{015F8240-2D6C-434D-A6FC-1A82D7D3B136}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Case 1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -70,9 +69,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,7 +390,7 @@
   <dimension ref="A1:C1126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,7 +418,7 @@
       <c r="A2">
         <v>672428360</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>6825874</v>
       </c>
       <c r="C2">

</xml_diff>